<commit_message>
Increased height and width of cells and allowed text wrapping
</commit_message>
<xml_diff>
--- a/new-schedule.xlsx
+++ b/new-schedule.xlsx
@@ -46,8 +46,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0" hidden="0"/>
@@ -413,71 +416,438 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E4"/>
+  <dimension ref="A1:F30"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <cols>
+    <col width="20" customWidth="1" min="1" max="1"/>
+    <col width="20" customWidth="1" min="2" max="2"/>
+    <col width="20" customWidth="1" min="3" max="3"/>
+    <col width="20" customWidth="1" min="4" max="4"/>
+    <col width="20" customWidth="1" min="5" max="5"/>
+    <col width="20" customWidth="1" min="6" max="6"/>
+  </cols>
   <sheetData>
-    <row r="1">
-      <c r="A1" t="inlineStr">
+    <row r="0" ht="50" customHeight="1"/>
+    <row r="1" ht="50" customHeight="1">
+      <c r="A1" s="1" t="n"/>
+      <c r="B1" s="1" t="inlineStr">
         <is>
           <t>Monday</t>
         </is>
       </c>
-      <c r="B1" t="inlineStr">
+      <c r="C1" s="1" t="inlineStr">
         <is>
           <t>Tuesday</t>
         </is>
       </c>
-      <c r="C1" t="inlineStr">
+      <c r="D1" s="1" t="inlineStr">
         <is>
           <t>Wednesday</t>
         </is>
       </c>
-      <c r="D1" t="inlineStr">
+      <c r="E1" s="1" t="inlineStr">
         <is>
           <t>Thursday</t>
         </is>
       </c>
-      <c r="E1" t="inlineStr">
+      <c r="F1" s="1" t="inlineStr">
         <is>
           <t>Friday</t>
         </is>
       </c>
     </row>
-    <row r="2">
-      <c r="A2" t="inlineStr">
-        <is>
-          <t>CPSC_V 221 - Basic Algorithms and Data Structures</t>
-        </is>
-      </c>
-      <c r="B2" t="inlineStr">
-        <is>
-          <t>MATH_V 200 - Calculus III</t>
-        </is>
-      </c>
-      <c r="D2" t="inlineStr">
-        <is>
-          <t>MATH_V 200 - Calculus III</t>
-        </is>
-      </c>
-    </row>
-    <row r="3">
-      <c r="D3" t="inlineStr">
-        <is>
-          <t>CPSC_V 330 - Applied Machine Learning</t>
-        </is>
-      </c>
-    </row>
-    <row r="4">
-      <c r="D4" t="inlineStr">
-        <is>
-          <t>EOSC_V 111 - Laboratory Exploration of Planet Earth</t>
-        </is>
-      </c>
+    <row r="2" ht="50" customHeight="1">
+      <c r="A2" s="1" t="inlineStr">
+        <is>
+          <t>8:00 a.m.</t>
+        </is>
+      </c>
+      <c r="B2" s="1" t="inlineStr">
+        <is>
+          <t>CPSC_V 221-101 - Basic Algorithms and Data Structures</t>
+        </is>
+      </c>
+      <c r="C2" s="1" t="inlineStr">
+        <is>
+          <t>MATH_V 200-102 - Calculus III</t>
+        </is>
+      </c>
+      <c r="D2" s="1" t="inlineStr">
+        <is>
+          <t>CPSC_V 221-101 - Basic Algorithms and Data Structures</t>
+        </is>
+      </c>
+      <c r="E2" s="1" t="inlineStr">
+        <is>
+          <t>MATH_V 200-102 - Calculus III</t>
+        </is>
+      </c>
+      <c r="F2" s="1" t="inlineStr">
+        <is>
+          <t>CPSC_V 221-101 - Basic Algorithms and Data Structures</t>
+        </is>
+      </c>
+    </row>
+    <row r="3" ht="50" customHeight="1">
+      <c r="A3" s="1" t="inlineStr">
+        <is>
+          <t>8:30 a.m.</t>
+        </is>
+      </c>
+      <c r="B3" s="1" t="inlineStr">
+        <is>
+          <t>CPSC_V 221-L1J - Basic Algorithms and Data Structures</t>
+        </is>
+      </c>
+      <c r="C3" s="1" t="inlineStr">
+        <is>
+          <t>CPSC_V 330-103 - Applied Machine Learning</t>
+        </is>
+      </c>
+      <c r="D3" s="1" t="n"/>
+      <c r="E3" s="1" t="inlineStr">
+        <is>
+          <t>CPSC_V 330-103 - Applied Machine Learning</t>
+        </is>
+      </c>
+      <c r="F3" s="1" t="n"/>
+    </row>
+    <row r="4" ht="50" customHeight="1">
+      <c r="A4" s="1" t="inlineStr">
+        <is>
+          <t>9:00 a.m.</t>
+        </is>
+      </c>
+      <c r="B4" s="1" t="n"/>
+      <c r="C4" s="1" t="n"/>
+      <c r="D4" s="1" t="n"/>
+      <c r="E4" s="1" t="inlineStr">
+        <is>
+          <t>CPSC_V 330-T1F - Applied Machine Learning</t>
+        </is>
+      </c>
+      <c r="F4" s="1" t="n"/>
+    </row>
+    <row r="5" ht="50" customHeight="1">
+      <c r="A5" s="1" t="inlineStr">
+        <is>
+          <t>9:30 a.m.</t>
+        </is>
+      </c>
+      <c r="B5" s="1" t="n"/>
+      <c r="C5" s="1" t="n"/>
+      <c r="D5" s="1" t="n"/>
+      <c r="E5" s="1" t="inlineStr">
+        <is>
+          <t>EOSC_V 111-L1E - Laboratory Exploration of Planet Earth</t>
+        </is>
+      </c>
+      <c r="F5" s="1" t="n"/>
+    </row>
+    <row r="6" ht="50" customHeight="1">
+      <c r="A6" s="1" t="inlineStr">
+        <is>
+          <t>10:00 a.m.</t>
+        </is>
+      </c>
+      <c r="B6" s="1" t="n"/>
+      <c r="C6" s="1" t="n"/>
+      <c r="D6" s="1" t="n"/>
+      <c r="E6" s="1" t="n"/>
+      <c r="F6" s="1" t="n"/>
+    </row>
+    <row r="7" ht="50" customHeight="1">
+      <c r="A7" s="1" t="inlineStr">
+        <is>
+          <t>10:30 a.m.</t>
+        </is>
+      </c>
+      <c r="B7" s="1" t="n"/>
+      <c r="C7" s="1" t="n"/>
+      <c r="D7" s="1" t="n"/>
+      <c r="E7" s="1" t="n"/>
+      <c r="F7" s="1" t="n"/>
+    </row>
+    <row r="8" ht="50" customHeight="1">
+      <c r="A8" s="1" t="inlineStr">
+        <is>
+          <t>11:00 a.m.</t>
+        </is>
+      </c>
+      <c r="B8" s="1" t="n"/>
+      <c r="C8" s="1" t="n"/>
+      <c r="D8" s="1" t="n"/>
+      <c r="E8" s="1" t="n"/>
+      <c r="F8" s="1" t="n"/>
+    </row>
+    <row r="9" ht="50" customHeight="1">
+      <c r="A9" s="1" t="inlineStr">
+        <is>
+          <t>11:30 a.m.</t>
+        </is>
+      </c>
+      <c r="B9" s="1" t="n"/>
+      <c r="C9" s="1" t="n"/>
+      <c r="D9" s="1" t="n"/>
+      <c r="E9" s="1" t="n"/>
+      <c r="F9" s="1" t="n"/>
+    </row>
+    <row r="10" ht="50" customHeight="1">
+      <c r="A10" s="1" t="inlineStr">
+        <is>
+          <t>12:00 p.m.</t>
+        </is>
+      </c>
+      <c r="B10" s="1" t="n"/>
+      <c r="C10" s="1" t="n"/>
+      <c r="D10" s="1" t="n"/>
+      <c r="E10" s="1" t="n"/>
+      <c r="F10" s="1" t="n"/>
+    </row>
+    <row r="11" ht="50" customHeight="1">
+      <c r="A11" s="1" t="inlineStr">
+        <is>
+          <t>12:30 p.m.</t>
+        </is>
+      </c>
+      <c r="B11" s="1" t="n"/>
+      <c r="C11" s="1" t="n"/>
+      <c r="D11" s="1" t="n"/>
+      <c r="E11" s="1" t="n"/>
+      <c r="F11" s="1" t="n"/>
+    </row>
+    <row r="12" ht="50" customHeight="1">
+      <c r="A12" s="1" t="inlineStr">
+        <is>
+          <t>1:00 p.m.</t>
+        </is>
+      </c>
+      <c r="B12" s="1" t="n"/>
+      <c r="C12" s="1" t="n"/>
+      <c r="D12" s="1" t="n"/>
+      <c r="E12" s="1" t="n"/>
+      <c r="F12" s="1" t="n"/>
+    </row>
+    <row r="13" ht="50" customHeight="1">
+      <c r="A13" s="1" t="inlineStr">
+        <is>
+          <t>1:30 p.m.</t>
+        </is>
+      </c>
+      <c r="B13" s="1" t="n"/>
+      <c r="C13" s="1" t="n"/>
+      <c r="D13" s="1" t="n"/>
+      <c r="E13" s="1" t="n"/>
+      <c r="F13" s="1" t="n"/>
+    </row>
+    <row r="14" ht="50" customHeight="1">
+      <c r="A14" s="1" t="inlineStr">
+        <is>
+          <t>2:00 p.m.</t>
+        </is>
+      </c>
+      <c r="B14" s="1" t="n"/>
+      <c r="C14" s="1" t="n"/>
+      <c r="D14" s="1" t="n"/>
+      <c r="E14" s="1" t="n"/>
+      <c r="F14" s="1" t="n"/>
+    </row>
+    <row r="15" ht="50" customHeight="1">
+      <c r="A15" s="1" t="inlineStr">
+        <is>
+          <t>2:30 p.m.</t>
+        </is>
+      </c>
+      <c r="B15" s="1" t="n"/>
+      <c r="C15" s="1" t="n"/>
+      <c r="D15" s="1" t="n"/>
+      <c r="E15" s="1" t="n"/>
+      <c r="F15" s="1" t="n"/>
+    </row>
+    <row r="16" ht="50" customHeight="1">
+      <c r="A16" s="1" t="inlineStr">
+        <is>
+          <t>3:00 p.m.</t>
+        </is>
+      </c>
+      <c r="B16" s="1" t="n"/>
+      <c r="C16" s="1" t="n"/>
+      <c r="D16" s="1" t="n"/>
+      <c r="E16" s="1" t="n"/>
+      <c r="F16" s="1" t="n"/>
+    </row>
+    <row r="17" ht="50" customHeight="1">
+      <c r="A17" s="1" t="inlineStr">
+        <is>
+          <t>3:30 p.m.</t>
+        </is>
+      </c>
+      <c r="B17" s="1" t="n"/>
+      <c r="C17" s="1" t="n"/>
+      <c r="D17" s="1" t="n"/>
+      <c r="E17" s="1" t="n"/>
+      <c r="F17" s="1" t="n"/>
+    </row>
+    <row r="18" ht="50" customHeight="1">
+      <c r="A18" s="1" t="inlineStr">
+        <is>
+          <t>4:00 p.m.</t>
+        </is>
+      </c>
+      <c r="B18" s="1" t="n"/>
+      <c r="C18" s="1" t="n"/>
+      <c r="D18" s="1" t="n"/>
+      <c r="E18" s="1" t="n"/>
+      <c r="F18" s="1" t="n"/>
+    </row>
+    <row r="19" ht="50" customHeight="1">
+      <c r="A19" s="1" t="inlineStr">
+        <is>
+          <t>4:30 p.m.</t>
+        </is>
+      </c>
+      <c r="B19" s="1" t="n"/>
+      <c r="C19" s="1" t="n"/>
+      <c r="D19" s="1" t="n"/>
+      <c r="E19" s="1" t="n"/>
+      <c r="F19" s="1" t="n"/>
+    </row>
+    <row r="20" ht="50" customHeight="1">
+      <c r="A20" s="1" t="inlineStr">
+        <is>
+          <t>5:00 p.m.</t>
+        </is>
+      </c>
+      <c r="B20" s="1" t="n"/>
+      <c r="C20" s="1" t="n"/>
+      <c r="D20" s="1" t="n"/>
+      <c r="E20" s="1" t="n"/>
+      <c r="F20" s="1" t="n"/>
+    </row>
+    <row r="21" ht="50" customHeight="1">
+      <c r="A21" s="1" t="inlineStr">
+        <is>
+          <t>5:30 p.m.</t>
+        </is>
+      </c>
+      <c r="B21" s="1" t="n"/>
+      <c r="C21" s="1" t="n"/>
+      <c r="D21" s="1" t="n"/>
+      <c r="E21" s="1" t="n"/>
+      <c r="F21" s="1" t="n"/>
+    </row>
+    <row r="22" ht="50" customHeight="1">
+      <c r="A22" s="1" t="inlineStr">
+        <is>
+          <t>6:00 p.m.</t>
+        </is>
+      </c>
+      <c r="B22" s="1" t="n"/>
+      <c r="C22" s="1" t="n"/>
+      <c r="D22" s="1" t="n"/>
+      <c r="E22" s="1" t="n"/>
+      <c r="F22" s="1" t="n"/>
+    </row>
+    <row r="23" ht="50" customHeight="1">
+      <c r="A23" s="1" t="inlineStr">
+        <is>
+          <t>6:30 p.m.</t>
+        </is>
+      </c>
+      <c r="B23" s="1" t="n"/>
+      <c r="C23" s="1" t="n"/>
+      <c r="D23" s="1" t="n"/>
+      <c r="E23" s="1" t="n"/>
+      <c r="F23" s="1" t="n"/>
+    </row>
+    <row r="24" ht="50" customHeight="1">
+      <c r="A24" s="1" t="inlineStr">
+        <is>
+          <t>7:00 p.m.</t>
+        </is>
+      </c>
+      <c r="B24" s="1" t="n"/>
+      <c r="C24" s="1" t="n"/>
+      <c r="D24" s="1" t="n"/>
+      <c r="E24" s="1" t="n"/>
+      <c r="F24" s="1" t="n"/>
+    </row>
+    <row r="25" ht="50" customHeight="1">
+      <c r="A25" s="1" t="inlineStr">
+        <is>
+          <t>7:30 p.m.</t>
+        </is>
+      </c>
+      <c r="B25" s="1" t="n"/>
+      <c r="C25" s="1" t="n"/>
+      <c r="D25" s="1" t="n"/>
+      <c r="E25" s="1" t="n"/>
+      <c r="F25" s="1" t="n"/>
+    </row>
+    <row r="26" ht="50" customHeight="1">
+      <c r="A26" s="1" t="inlineStr">
+        <is>
+          <t>8:00 p.m.</t>
+        </is>
+      </c>
+      <c r="B26" s="1" t="n"/>
+      <c r="C26" s="1" t="n"/>
+      <c r="D26" s="1" t="n"/>
+      <c r="E26" s="1" t="n"/>
+      <c r="F26" s="1" t="n"/>
+    </row>
+    <row r="27" ht="50" customHeight="1">
+      <c r="A27" s="1" t="inlineStr">
+        <is>
+          <t>8:30 p.m.</t>
+        </is>
+      </c>
+      <c r="B27" s="1" t="n"/>
+      <c r="C27" s="1" t="n"/>
+      <c r="D27" s="1" t="n"/>
+      <c r="E27" s="1" t="n"/>
+      <c r="F27" s="1" t="n"/>
+    </row>
+    <row r="28" ht="50" customHeight="1">
+      <c r="A28" s="1" t="inlineStr">
+        <is>
+          <t>9:00 p.m.</t>
+        </is>
+      </c>
+      <c r="B28" s="1" t="n"/>
+      <c r="C28" s="1" t="n"/>
+      <c r="D28" s="1" t="n"/>
+      <c r="E28" s="1" t="n"/>
+      <c r="F28" s="1" t="n"/>
+    </row>
+    <row r="29" ht="50" customHeight="1">
+      <c r="A29" s="1" t="inlineStr">
+        <is>
+          <t>9:30 p.m.</t>
+        </is>
+      </c>
+      <c r="B29" s="1" t="n"/>
+      <c r="C29" s="1" t="n"/>
+      <c r="D29" s="1" t="n"/>
+      <c r="E29" s="1" t="n"/>
+      <c r="F29" s="1" t="n"/>
+    </row>
+    <row r="30">
+      <c r="A30" s="1" t="inlineStr">
+        <is>
+          <t>10:00 p.m.</t>
+        </is>
+      </c>
+      <c r="B30" s="1" t="n"/>
+      <c r="C30" s="1" t="n"/>
+      <c r="D30" s="1" t="n"/>
+      <c r="E30" s="1" t="n"/>
+      <c r="F30" s="1" t="n"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>

<commit_message>
Cells now merge when classes are displayed on the schedule
</commit_message>
<xml_diff>
--- a/new-schedule.xlsx
+++ b/new-schedule.xlsx
@@ -432,8 +432,8 @@
     <col width="20" customWidth="1" min="6" max="6"/>
   </cols>
   <sheetData>
-    <row r="0" ht="50" customHeight="1"/>
-    <row r="1" ht="50" customHeight="1">
+    <row r="0" ht="20" customHeight="1"/>
+    <row r="1" ht="20" customHeight="1">
       <c r="A1" s="1" t="n"/>
       <c r="B1" s="1" t="inlineStr">
         <is>
@@ -461,79 +461,53 @@
         </is>
       </c>
     </row>
-    <row r="2" ht="50" customHeight="1">
+    <row r="2" ht="20" customHeight="1">
       <c r="A2" s="1" t="inlineStr">
         <is>
           <t>8:00 a.m.</t>
         </is>
       </c>
-      <c r="B2" s="1" t="inlineStr">
-        <is>
-          <t>CPSC_V 221-101 - Basic Algorithms and Data Structures</t>
-        </is>
-      </c>
-      <c r="C2" s="1" t="inlineStr">
-        <is>
-          <t>MATH_V 200-102 - Calculus III</t>
-        </is>
-      </c>
-      <c r="D2" s="1" t="inlineStr">
-        <is>
-          <t>CPSC_V 221-101 - Basic Algorithms and Data Structures</t>
-        </is>
-      </c>
+      <c r="B2" s="1" t="n"/>
+      <c r="C2" s="1" t="n"/>
+      <c r="D2" s="1" t="n"/>
       <c r="E2" s="1" t="inlineStr">
         <is>
-          <t>MATH_V 200-102 - Calculus III</t>
-        </is>
-      </c>
-      <c r="F2" s="1" t="inlineStr">
-        <is>
-          <t>CPSC_V 221-101 - Basic Algorithms and Data Structures</t>
-        </is>
-      </c>
-    </row>
-    <row r="3" ht="50" customHeight="1">
+          <t>EOSC_V 111-L1E - Laboratory Exploration of Planet Earth
+8:00 a.m. - 11:00 a.m.</t>
+        </is>
+      </c>
+      <c r="F2" s="1" t="n"/>
+    </row>
+    <row r="3" ht="20" customHeight="1">
       <c r="A3" s="1" t="inlineStr">
         <is>
           <t>8:30 a.m.</t>
         </is>
       </c>
-      <c r="B3" s="1" t="inlineStr">
-        <is>
-          <t>CPSC_V 221-L1J - Basic Algorithms and Data Structures</t>
-        </is>
-      </c>
-      <c r="C3" s="1" t="inlineStr">
-        <is>
-          <t>CPSC_V 330-103 - Applied Machine Learning</t>
-        </is>
-      </c>
+      <c r="B3" s="1" t="n"/>
+      <c r="C3" s="1" t="n"/>
       <c r="D3" s="1" t="n"/>
-      <c r="E3" s="1" t="inlineStr">
-        <is>
-          <t>CPSC_V 330-103 - Applied Machine Learning</t>
-        </is>
-      </c>
+      <c r="E3" s="1" t="n"/>
       <c r="F3" s="1" t="n"/>
     </row>
-    <row r="4" ht="50" customHeight="1">
+    <row r="4" ht="20" customHeight="1">
       <c r="A4" s="1" t="inlineStr">
         <is>
           <t>9:00 a.m.</t>
         </is>
       </c>
-      <c r="B4" s="1" t="n"/>
+      <c r="B4" s="1" t="inlineStr">
+        <is>
+          <t>CPSC_V 221-L1J - Basic Algorithms and Data Structures
+9:00 a.m. - 11:00 a.m.</t>
+        </is>
+      </c>
       <c r="C4" s="1" t="n"/>
       <c r="D4" s="1" t="n"/>
-      <c r="E4" s="1" t="inlineStr">
-        <is>
-          <t>CPSC_V 330-T1F - Applied Machine Learning</t>
-        </is>
-      </c>
+      <c r="E4" s="1" t="n"/>
       <c r="F4" s="1" t="n"/>
     </row>
-    <row r="5" ht="50" customHeight="1">
+    <row r="5" ht="20" customHeight="1">
       <c r="A5" s="1" t="inlineStr">
         <is>
           <t>9:30 a.m.</t>
@@ -542,14 +516,10 @@
       <c r="B5" s="1" t="n"/>
       <c r="C5" s="1" t="n"/>
       <c r="D5" s="1" t="n"/>
-      <c r="E5" s="1" t="inlineStr">
-        <is>
-          <t>EOSC_V 111-L1E - Laboratory Exploration of Planet Earth</t>
-        </is>
-      </c>
+      <c r="E5" s="1" t="n"/>
       <c r="F5" s="1" t="n"/>
     </row>
-    <row r="6" ht="50" customHeight="1">
+    <row r="6" ht="20" customHeight="1">
       <c r="A6" s="1" t="inlineStr">
         <is>
           <t>10:00 a.m.</t>
@@ -561,7 +531,7 @@
       <c r="E6" s="1" t="n"/>
       <c r="F6" s="1" t="n"/>
     </row>
-    <row r="7" ht="50" customHeight="1">
+    <row r="7" ht="20" customHeight="1">
       <c r="A7" s="1" t="inlineStr">
         <is>
           <t>10:30 a.m.</t>
@@ -573,19 +543,29 @@
       <c r="E7" s="1" t="n"/>
       <c r="F7" s="1" t="n"/>
     </row>
-    <row r="8" ht="50" customHeight="1">
+    <row r="8" ht="20" customHeight="1">
       <c r="A8" s="1" t="inlineStr">
         <is>
           <t>11:00 a.m.</t>
         </is>
       </c>
       <c r="B8" s="1" t="n"/>
-      <c r="C8" s="1" t="n"/>
+      <c r="C8" s="1" t="inlineStr">
+        <is>
+          <t>MATH_V 200-102 - Calculus III
+11:00 a.m. - 12:30 p.m.</t>
+        </is>
+      </c>
       <c r="D8" s="1" t="n"/>
-      <c r="E8" s="1" t="n"/>
+      <c r="E8" s="1" t="inlineStr">
+        <is>
+          <t>MATH_V 200-102 - Calculus III
+11:00 a.m. - 12:30 p.m.</t>
+        </is>
+      </c>
       <c r="F8" s="1" t="n"/>
     </row>
-    <row r="9" ht="50" customHeight="1">
+    <row r="9" ht="20" customHeight="1">
       <c r="A9" s="1" t="inlineStr">
         <is>
           <t>11:30 a.m.</t>
@@ -597,7 +577,7 @@
       <c r="E9" s="1" t="n"/>
       <c r="F9" s="1" t="n"/>
     </row>
-    <row r="10" ht="50" customHeight="1">
+    <row r="10" ht="20" customHeight="1">
       <c r="A10" s="1" t="inlineStr">
         <is>
           <t>12:00 p.m.</t>
@@ -609,7 +589,7 @@
       <c r="E10" s="1" t="n"/>
       <c r="F10" s="1" t="n"/>
     </row>
-    <row r="11" ht="50" customHeight="1">
+    <row r="11" ht="20" customHeight="1">
       <c r="A11" s="1" t="inlineStr">
         <is>
           <t>12:30 p.m.</t>
@@ -621,7 +601,7 @@
       <c r="E11" s="1" t="n"/>
       <c r="F11" s="1" t="n"/>
     </row>
-    <row r="12" ht="50" customHeight="1">
+    <row r="12" ht="20" customHeight="1">
       <c r="A12" s="1" t="inlineStr">
         <is>
           <t>1:00 p.m.</t>
@@ -630,10 +610,15 @@
       <c r="B12" s="1" t="n"/>
       <c r="C12" s="1" t="n"/>
       <c r="D12" s="1" t="n"/>
-      <c r="E12" s="1" t="n"/>
+      <c r="E12" s="1" t="inlineStr">
+        <is>
+          <t>CPSC_V 330-T1F - Applied Machine Learning
+1:00 p.m. - 2:00 p.m.</t>
+        </is>
+      </c>
       <c r="F12" s="1" t="n"/>
     </row>
-    <row r="13" ht="50" customHeight="1">
+    <row r="13" ht="20" customHeight="1">
       <c r="A13" s="1" t="inlineStr">
         <is>
           <t>1:30 p.m.</t>
@@ -645,19 +630,34 @@
       <c r="E13" s="1" t="n"/>
       <c r="F13" s="1" t="n"/>
     </row>
-    <row r="14" ht="50" customHeight="1">
+    <row r="14" ht="20" customHeight="1">
       <c r="A14" s="1" t="inlineStr">
         <is>
           <t>2:00 p.m.</t>
         </is>
       </c>
-      <c r="B14" s="1" t="n"/>
+      <c r="B14" s="1" t="inlineStr">
+        <is>
+          <t>CPSC_V 221-101 - Basic Algorithms and Data Structures
+2:00 p.m. - 3:00 p.m.</t>
+        </is>
+      </c>
       <c r="C14" s="1" t="n"/>
-      <c r="D14" s="1" t="n"/>
+      <c r="D14" s="1" t="inlineStr">
+        <is>
+          <t>CPSC_V 221-101 - Basic Algorithms and Data Structures
+2:00 p.m. - 3:00 p.m.</t>
+        </is>
+      </c>
       <c r="E14" s="1" t="n"/>
-      <c r="F14" s="1" t="n"/>
-    </row>
-    <row r="15" ht="50" customHeight="1">
+      <c r="F14" s="1" t="inlineStr">
+        <is>
+          <t>CPSC_V 221-101 - Basic Algorithms and Data Structures
+2:00 p.m. - 3:00 p.m.</t>
+        </is>
+      </c>
+    </row>
+    <row r="15" ht="20" customHeight="1">
       <c r="A15" s="1" t="inlineStr">
         <is>
           <t>2:30 p.m.</t>
@@ -669,7 +669,7 @@
       <c r="E15" s="1" t="n"/>
       <c r="F15" s="1" t="n"/>
     </row>
-    <row r="16" ht="50" customHeight="1">
+    <row r="16" ht="20" customHeight="1">
       <c r="A16" s="1" t="inlineStr">
         <is>
           <t>3:00 p.m.</t>
@@ -681,7 +681,7 @@
       <c r="E16" s="1" t="n"/>
       <c r="F16" s="1" t="n"/>
     </row>
-    <row r="17" ht="50" customHeight="1">
+    <row r="17" ht="20" customHeight="1">
       <c r="A17" s="1" t="inlineStr">
         <is>
           <t>3:30 p.m.</t>
@@ -693,7 +693,7 @@
       <c r="E17" s="1" t="n"/>
       <c r="F17" s="1" t="n"/>
     </row>
-    <row r="18" ht="50" customHeight="1">
+    <row r="18" ht="20" customHeight="1">
       <c r="A18" s="1" t="inlineStr">
         <is>
           <t>4:00 p.m.</t>
@@ -705,7 +705,7 @@
       <c r="E18" s="1" t="n"/>
       <c r="F18" s="1" t="n"/>
     </row>
-    <row r="19" ht="50" customHeight="1">
+    <row r="19" ht="20" customHeight="1">
       <c r="A19" s="1" t="inlineStr">
         <is>
           <t>4:30 p.m.</t>
@@ -717,19 +717,29 @@
       <c r="E19" s="1" t="n"/>
       <c r="F19" s="1" t="n"/>
     </row>
-    <row r="20" ht="50" customHeight="1">
+    <row r="20" ht="20" customHeight="1">
       <c r="A20" s="1" t="inlineStr">
         <is>
           <t>5:00 p.m.</t>
         </is>
       </c>
       <c r="B20" s="1" t="n"/>
-      <c r="C20" s="1" t="n"/>
+      <c r="C20" s="1" t="inlineStr">
+        <is>
+          <t>CPSC_V 330-103 - Applied Machine Learning
+5:00 p.m. - 6:30 p.m.</t>
+        </is>
+      </c>
       <c r="D20" s="1" t="n"/>
-      <c r="E20" s="1" t="n"/>
+      <c r="E20" s="1" t="inlineStr">
+        <is>
+          <t>CPSC_V 330-103 - Applied Machine Learning
+5:00 p.m. - 6:30 p.m.</t>
+        </is>
+      </c>
       <c r="F20" s="1" t="n"/>
     </row>
-    <row r="21" ht="50" customHeight="1">
+    <row r="21" ht="20" customHeight="1">
       <c r="A21" s="1" t="inlineStr">
         <is>
           <t>5:30 p.m.</t>
@@ -741,7 +751,7 @@
       <c r="E21" s="1" t="n"/>
       <c r="F21" s="1" t="n"/>
     </row>
-    <row r="22" ht="50" customHeight="1">
+    <row r="22" ht="20" customHeight="1">
       <c r="A22" s="1" t="inlineStr">
         <is>
           <t>6:00 p.m.</t>
@@ -753,7 +763,7 @@
       <c r="E22" s="1" t="n"/>
       <c r="F22" s="1" t="n"/>
     </row>
-    <row r="23" ht="50" customHeight="1">
+    <row r="23" ht="20" customHeight="1">
       <c r="A23" s="1" t="inlineStr">
         <is>
           <t>6:30 p.m.</t>
@@ -765,7 +775,7 @@
       <c r="E23" s="1" t="n"/>
       <c r="F23" s="1" t="n"/>
     </row>
-    <row r="24" ht="50" customHeight="1">
+    <row r="24" ht="20" customHeight="1">
       <c r="A24" s="1" t="inlineStr">
         <is>
           <t>7:00 p.m.</t>
@@ -777,7 +787,7 @@
       <c r="E24" s="1" t="n"/>
       <c r="F24" s="1" t="n"/>
     </row>
-    <row r="25" ht="50" customHeight="1">
+    <row r="25" ht="20" customHeight="1">
       <c r="A25" s="1" t="inlineStr">
         <is>
           <t>7:30 p.m.</t>
@@ -789,7 +799,7 @@
       <c r="E25" s="1" t="n"/>
       <c r="F25" s="1" t="n"/>
     </row>
-    <row r="26" ht="50" customHeight="1">
+    <row r="26" ht="20" customHeight="1">
       <c r="A26" s="1" t="inlineStr">
         <is>
           <t>8:00 p.m.</t>
@@ -801,7 +811,7 @@
       <c r="E26" s="1" t="n"/>
       <c r="F26" s="1" t="n"/>
     </row>
-    <row r="27" ht="50" customHeight="1">
+    <row r="27" ht="20" customHeight="1">
       <c r="A27" s="1" t="inlineStr">
         <is>
           <t>8:30 p.m.</t>
@@ -813,7 +823,7 @@
       <c r="E27" s="1" t="n"/>
       <c r="F27" s="1" t="n"/>
     </row>
-    <row r="28" ht="50" customHeight="1">
+    <row r="28" ht="20" customHeight="1">
       <c r="A28" s="1" t="inlineStr">
         <is>
           <t>9:00 p.m.</t>
@@ -825,7 +835,7 @@
       <c r="E28" s="1" t="n"/>
       <c r="F28" s="1" t="n"/>
     </row>
-    <row r="29" ht="50" customHeight="1">
+    <row r="29" ht="20" customHeight="1">
       <c r="A29" s="1" t="inlineStr">
         <is>
           <t>9:30 p.m.</t>
@@ -838,18 +848,25 @@
       <c r="F29" s="1" t="n"/>
     </row>
     <row r="30">
-      <c r="A30" s="1" t="inlineStr">
+      <c r="A30" t="inlineStr">
         <is>
           <t>10:00 p.m.</t>
         </is>
       </c>
-      <c r="B30" s="1" t="n"/>
-      <c r="C30" s="1" t="n"/>
-      <c r="D30" s="1" t="n"/>
-      <c r="E30" s="1" t="n"/>
-      <c r="F30" s="1" t="n"/>
     </row>
   </sheetData>
+  <mergeCells count="10">
+    <mergeCell ref="E8:E10"/>
+    <mergeCell ref="B4:B7"/>
+    <mergeCell ref="E12:E13"/>
+    <mergeCell ref="C20:C22"/>
+    <mergeCell ref="E20:E22"/>
+    <mergeCell ref="E2:E7"/>
+    <mergeCell ref="C8:C10"/>
+    <mergeCell ref="D14:D15"/>
+    <mergeCell ref="B14:B15"/>
+    <mergeCell ref="F14:F15"/>
+  </mergeCells>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Allows users to upload excel files on HTML website and choose term numbers to create a term schedule.
</commit_message>
<xml_diff>
--- a/new-schedule.xlsx
+++ b/new-schedule.xlsx
@@ -46,8 +46,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="general" vertical="top"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment wrapText="1"/>
     </xf>
@@ -424,448 +427,453 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <cols>
-    <col width="20" customWidth="1" min="1" max="1"/>
-    <col width="20" customWidth="1" min="2" max="2"/>
-    <col width="20" customWidth="1" min="3" max="3"/>
-    <col width="20" customWidth="1" min="4" max="4"/>
-    <col width="20" customWidth="1" min="5" max="5"/>
-    <col width="20" customWidth="1" min="6" max="6"/>
+    <col width="25" customWidth="1" min="1" max="1"/>
+    <col width="25" customWidth="1" min="2" max="2"/>
+    <col width="25" customWidth="1" min="3" max="3"/>
+    <col width="25" customWidth="1" min="4" max="4"/>
+    <col width="25" customWidth="1" min="5" max="5"/>
+    <col width="25" customWidth="1" min="6" max="6"/>
   </cols>
   <sheetData>
-    <row r="0" ht="20" customHeight="1"/>
-    <row r="1" ht="20" customHeight="1">
+    <row r="0" ht="30" customHeight="1"/>
+    <row r="1" ht="30" customHeight="1">
       <c r="A1" s="1" t="n"/>
-      <c r="B1" s="1" t="inlineStr">
+      <c r="B1" s="2" t="inlineStr">
         <is>
           <t>Monday</t>
         </is>
       </c>
-      <c r="C1" s="1" t="inlineStr">
+      <c r="C1" s="2" t="inlineStr">
         <is>
           <t>Tuesday</t>
         </is>
       </c>
-      <c r="D1" s="1" t="inlineStr">
+      <c r="D1" s="2" t="inlineStr">
         <is>
           <t>Wednesday</t>
         </is>
       </c>
-      <c r="E1" s="1" t="inlineStr">
+      <c r="E1" s="2" t="inlineStr">
         <is>
           <t>Thursday</t>
         </is>
       </c>
-      <c r="F1" s="1" t="inlineStr">
+      <c r="F1" s="2" t="inlineStr">
         <is>
           <t>Friday</t>
         </is>
       </c>
     </row>
-    <row r="2" ht="20" customHeight="1">
+    <row r="2" ht="30" customHeight="1">
       <c r="A2" s="1" t="inlineStr">
         <is>
           <t>8:00 a.m.</t>
         </is>
       </c>
-      <c r="B2" s="1" t="n"/>
-      <c r="C2" s="1" t="n"/>
-      <c r="D2" s="1" t="n"/>
-      <c r="E2" s="1" t="inlineStr">
-        <is>
-          <t>EOSC_V 111-L1E - Laboratory Exploration of Planet Earth
-8:00 a.m. - 11:00 a.m.</t>
-        </is>
-      </c>
-      <c r="F2" s="1" t="n"/>
-    </row>
-    <row r="3" ht="20" customHeight="1">
+      <c r="B2" s="2" t="n"/>
+      <c r="C2" s="2" t="n"/>
+      <c r="D2" s="2" t="n"/>
+      <c r="E2" s="2" t="n"/>
+      <c r="F2" s="2" t="n"/>
+    </row>
+    <row r="3" ht="30" customHeight="1">
       <c r="A3" s="1" t="inlineStr">
         <is>
           <t>8:30 a.m.</t>
         </is>
       </c>
-      <c r="B3" s="1" t="n"/>
-      <c r="C3" s="1" t="n"/>
-      <c r="D3" s="1" t="n"/>
-      <c r="E3" s="1" t="n"/>
-      <c r="F3" s="1" t="n"/>
-    </row>
-    <row r="4" ht="20" customHeight="1">
+      <c r="B3" s="2" t="n"/>
+      <c r="C3" s="2" t="n"/>
+      <c r="D3" s="2" t="n"/>
+      <c r="E3" s="2" t="n"/>
+      <c r="F3" s="2" t="n"/>
+    </row>
+    <row r="4" ht="30" customHeight="1">
       <c r="A4" s="1" t="inlineStr">
         <is>
           <t>9:00 a.m.</t>
         </is>
       </c>
-      <c r="B4" s="1" t="inlineStr">
-        <is>
-          <t>CPSC_V 221-L1J - Basic Algorithms and Data Structures
-9:00 a.m. - 11:00 a.m.</t>
-        </is>
-      </c>
-      <c r="C4" s="1" t="n"/>
-      <c r="D4" s="1" t="n"/>
-      <c r="E4" s="1" t="n"/>
-      <c r="F4" s="1" t="n"/>
-    </row>
-    <row r="5" ht="20" customHeight="1">
+      <c r="B4" s="2" t="n"/>
+      <c r="C4" s="2" t="n"/>
+      <c r="D4" s="2" t="n"/>
+      <c r="E4" s="2" t="n"/>
+      <c r="F4" s="2" t="n"/>
+    </row>
+    <row r="5" ht="30" customHeight="1">
       <c r="A5" s="1" t="inlineStr">
         <is>
           <t>9:30 a.m.</t>
         </is>
       </c>
-      <c r="B5" s="1" t="n"/>
-      <c r="C5" s="1" t="n"/>
-      <c r="D5" s="1" t="n"/>
-      <c r="E5" s="1" t="n"/>
-      <c r="F5" s="1" t="n"/>
-    </row>
-    <row r="6" ht="20" customHeight="1">
+      <c r="B5" s="2" t="n"/>
+      <c r="C5" s="2" t="n"/>
+      <c r="D5" s="2" t="n"/>
+      <c r="E5" s="2" t="n"/>
+      <c r="F5" s="2" t="n"/>
+    </row>
+    <row r="6" ht="30" customHeight="1">
       <c r="A6" s="1" t="inlineStr">
         <is>
           <t>10:00 a.m.</t>
         </is>
       </c>
-      <c r="B6" s="1" t="n"/>
-      <c r="C6" s="1" t="n"/>
-      <c r="D6" s="1" t="n"/>
-      <c r="E6" s="1" t="n"/>
-      <c r="F6" s="1" t="n"/>
-    </row>
-    <row r="7" ht="20" customHeight="1">
+      <c r="B6" s="2" t="n"/>
+      <c r="C6" s="2" t="inlineStr">
+        <is>
+          <t>CPSC_V 213-L2F - Introduction to Computer Systems
+10:00 a.m. - 11:00 a.m.</t>
+        </is>
+      </c>
+      <c r="D6" s="2" t="n"/>
+      <c r="E6" s="2" t="inlineStr">
+        <is>
+          <t>CPSC_V 213-L2F - Introduction to Computer Systems
+10:00 a.m. - 11:00 a.m.</t>
+        </is>
+      </c>
+      <c r="F6" s="2" t="n"/>
+    </row>
+    <row r="7" ht="30" customHeight="1">
       <c r="A7" s="1" t="inlineStr">
         <is>
           <t>10:30 a.m.</t>
         </is>
       </c>
-      <c r="B7" s="1" t="n"/>
-      <c r="C7" s="1" t="n"/>
-      <c r="D7" s="1" t="n"/>
-      <c r="E7" s="1" t="n"/>
-      <c r="F7" s="1" t="n"/>
-    </row>
-    <row r="8" ht="20" customHeight="1">
+      <c r="B7" s="2" t="n"/>
+      <c r="C7" s="2" t="n"/>
+      <c r="D7" s="2" t="n"/>
+      <c r="E7" s="2" t="n"/>
+      <c r="F7" s="2" t="n"/>
+    </row>
+    <row r="8" ht="30" customHeight="1">
       <c r="A8" s="1" t="inlineStr">
         <is>
           <t>11:00 a.m.</t>
         </is>
       </c>
-      <c r="B8" s="1" t="n"/>
-      <c r="C8" s="1" t="inlineStr">
-        <is>
-          <t>MATH_V 200-102 - Calculus III
-11:00 a.m. - 12:30 p.m.</t>
-        </is>
-      </c>
-      <c r="D8" s="1" t="n"/>
-      <c r="E8" s="1" t="inlineStr">
-        <is>
-          <t>MATH_V 200-102 - Calculus III
-11:00 a.m. - 12:30 p.m.</t>
-        </is>
-      </c>
-      <c r="F8" s="1" t="n"/>
-    </row>
-    <row r="9" ht="20" customHeight="1">
+      <c r="B8" s="2" t="inlineStr">
+        <is>
+          <t>CPSC_V 213-205 - Introduction to Computer Systems
+11:00 a.m. - 12:00 p.m.</t>
+        </is>
+      </c>
+      <c r="C8" s="2" t="n"/>
+      <c r="D8" s="2" t="inlineStr">
+        <is>
+          <t>CPSC_V 213-205 - Introduction to Computer Systems
+11:00 a.m. - 12:00 p.m.</t>
+        </is>
+      </c>
+      <c r="E8" s="2" t="n"/>
+      <c r="F8" s="2" t="inlineStr">
+        <is>
+          <t>CPSC_V 213-205 - Introduction to Computer Systems
+11:00 a.m. - 12:00 p.m.</t>
+        </is>
+      </c>
+    </row>
+    <row r="9" ht="30" customHeight="1">
       <c r="A9" s="1" t="inlineStr">
         <is>
           <t>11:30 a.m.</t>
         </is>
       </c>
-      <c r="B9" s="1" t="n"/>
-      <c r="C9" s="1" t="n"/>
-      <c r="D9" s="1" t="n"/>
-      <c r="E9" s="1" t="n"/>
-      <c r="F9" s="1" t="n"/>
-    </row>
-    <row r="10" ht="20" customHeight="1">
+      <c r="B9" s="2" t="n"/>
+      <c r="C9" s="2" t="n"/>
+      <c r="D9" s="2" t="n"/>
+      <c r="E9" s="2" t="n"/>
+      <c r="F9" s="2" t="n"/>
+    </row>
+    <row r="10" ht="30" customHeight="1">
       <c r="A10" s="1" t="inlineStr">
         <is>
           <t>12:00 p.m.</t>
         </is>
       </c>
-      <c r="B10" s="1" t="n"/>
-      <c r="C10" s="1" t="n"/>
-      <c r="D10" s="1" t="n"/>
-      <c r="E10" s="1" t="n"/>
-      <c r="F10" s="1" t="n"/>
-    </row>
-    <row r="11" ht="20" customHeight="1">
+      <c r="B10" s="2" t="n"/>
+      <c r="C10" s="2" t="n"/>
+      <c r="D10" s="2" t="n"/>
+      <c r="E10" s="2" t="n"/>
+      <c r="F10" s="2" t="n"/>
+    </row>
+    <row r="11" ht="30" customHeight="1">
       <c r="A11" s="1" t="inlineStr">
         <is>
           <t>12:30 p.m.</t>
         </is>
       </c>
-      <c r="B11" s="1" t="n"/>
-      <c r="C11" s="1" t="n"/>
-      <c r="D11" s="1" t="n"/>
-      <c r="E11" s="1" t="n"/>
-      <c r="F11" s="1" t="n"/>
-    </row>
-    <row r="12" ht="20" customHeight="1">
+      <c r="B11" s="2" t="n"/>
+      <c r="C11" s="2" t="inlineStr">
+        <is>
+          <t>MATH_V 221-202 - Matrix Algebra
+12:30 p.m. - 2:00 p.m.</t>
+        </is>
+      </c>
+      <c r="D11" s="2" t="n"/>
+      <c r="E11" s="2" t="inlineStr">
+        <is>
+          <t>MATH_V 221-202 - Matrix Algebra
+12:30 p.m. - 2:00 p.m.</t>
+        </is>
+      </c>
+      <c r="F11" s="2" t="n"/>
+    </row>
+    <row r="12" ht="30" customHeight="1">
       <c r="A12" s="1" t="inlineStr">
         <is>
           <t>1:00 p.m.</t>
         </is>
       </c>
-      <c r="B12" s="1" t="n"/>
-      <c r="C12" s="1" t="n"/>
-      <c r="D12" s="1" t="n"/>
-      <c r="E12" s="1" t="inlineStr">
-        <is>
-          <t>CPSC_V 330-T1F - Applied Machine Learning
+      <c r="B12" s="2" t="inlineStr">
+        <is>
+          <t>ENGL_V 110-010 - Approaches to Literature and Culture
 1:00 p.m. - 2:00 p.m.</t>
         </is>
       </c>
-      <c r="F12" s="1" t="n"/>
-    </row>
-    <row r="13" ht="20" customHeight="1">
+      <c r="C12" s="2" t="n"/>
+      <c r="D12" s="2" t="inlineStr">
+        <is>
+          <t>ENGL_V 110-010 - Approaches to Literature and Culture
+1:00 p.m. - 2:00 p.m.</t>
+        </is>
+      </c>
+      <c r="E12" s="2" t="n"/>
+      <c r="F12" s="2" t="inlineStr">
+        <is>
+          <t>ENGL_V 110-LS1 - Approaches to Literature and Culture
+1:00 p.m. - 2:00 p.m.</t>
+        </is>
+      </c>
+    </row>
+    <row r="13" ht="30" customHeight="1">
       <c r="A13" s="1" t="inlineStr">
         <is>
           <t>1:30 p.m.</t>
         </is>
       </c>
-      <c r="B13" s="1" t="n"/>
-      <c r="C13" s="1" t="n"/>
-      <c r="D13" s="1" t="n"/>
-      <c r="E13" s="1" t="n"/>
-      <c r="F13" s="1" t="n"/>
-    </row>
-    <row r="14" ht="20" customHeight="1">
+      <c r="B13" s="2" t="n"/>
+      <c r="C13" s="2" t="n"/>
+      <c r="D13" s="2" t="n"/>
+      <c r="E13" s="2" t="n"/>
+      <c r="F13" s="2" t="n"/>
+    </row>
+    <row r="14" ht="30" customHeight="1">
       <c r="A14" s="1" t="inlineStr">
         <is>
           <t>2:00 p.m.</t>
         </is>
       </c>
-      <c r="B14" s="1" t="inlineStr">
-        <is>
-          <t>CPSC_V 221-101 - Basic Algorithms and Data Structures
-2:00 p.m. - 3:00 p.m.</t>
-        </is>
-      </c>
-      <c r="C14" s="1" t="n"/>
-      <c r="D14" s="1" t="inlineStr">
-        <is>
-          <t>CPSC_V 221-101 - Basic Algorithms and Data Structures
-2:00 p.m. - 3:00 p.m.</t>
-        </is>
-      </c>
-      <c r="E14" s="1" t="n"/>
-      <c r="F14" s="1" t="inlineStr">
-        <is>
-          <t>CPSC_V 221-101 - Basic Algorithms and Data Structures
-2:00 p.m. - 3:00 p.m.</t>
-        </is>
-      </c>
-    </row>
-    <row r="15" ht="20" customHeight="1">
+      <c r="B14" s="2" t="n"/>
+      <c r="C14" s="2" t="n"/>
+      <c r="D14" s="2" t="n"/>
+      <c r="E14" s="2" t="n"/>
+      <c r="F14" s="2" t="n"/>
+    </row>
+    <row r="15" ht="30" customHeight="1">
       <c r="A15" s="1" t="inlineStr">
         <is>
           <t>2:30 p.m.</t>
         </is>
       </c>
-      <c r="B15" s="1" t="n"/>
-      <c r="C15" s="1" t="n"/>
-      <c r="D15" s="1" t="n"/>
-      <c r="E15" s="1" t="n"/>
-      <c r="F15" s="1" t="n"/>
-    </row>
-    <row r="16" ht="20" customHeight="1">
+      <c r="B15" s="2" t="n"/>
+      <c r="C15" s="2" t="n"/>
+      <c r="D15" s="2" t="n"/>
+      <c r="E15" s="2" t="n"/>
+      <c r="F15" s="2" t="n"/>
+    </row>
+    <row r="16" ht="30" customHeight="1">
       <c r="A16" s="1" t="inlineStr">
         <is>
           <t>3:00 p.m.</t>
         </is>
       </c>
-      <c r="B16" s="1" t="n"/>
-      <c r="C16" s="1" t="n"/>
-      <c r="D16" s="1" t="n"/>
-      <c r="E16" s="1" t="n"/>
-      <c r="F16" s="1" t="n"/>
-    </row>
-    <row r="17" ht="20" customHeight="1">
+      <c r="B16" s="2" t="n"/>
+      <c r="C16" s="2" t="n"/>
+      <c r="D16" s="2" t="n"/>
+      <c r="E16" s="2" t="n"/>
+      <c r="F16" s="2" t="n"/>
+    </row>
+    <row r="17" ht="30" customHeight="1">
       <c r="A17" s="1" t="inlineStr">
         <is>
           <t>3:30 p.m.</t>
         </is>
       </c>
-      <c r="B17" s="1" t="n"/>
-      <c r="C17" s="1" t="n"/>
-      <c r="D17" s="1" t="n"/>
-      <c r="E17" s="1" t="n"/>
-      <c r="F17" s="1" t="n"/>
-    </row>
-    <row r="18" ht="20" customHeight="1">
+      <c r="B17" s="2" t="n"/>
+      <c r="C17" s="2" t="n"/>
+      <c r="D17" s="2" t="n"/>
+      <c r="E17" s="2" t="n"/>
+      <c r="F17" s="2" t="n"/>
+    </row>
+    <row r="18" ht="30" customHeight="1">
       <c r="A18" s="1" t="inlineStr">
         <is>
           <t>4:00 p.m.</t>
         </is>
       </c>
-      <c r="B18" s="1" t="n"/>
-      <c r="C18" s="1" t="n"/>
-      <c r="D18" s="1" t="n"/>
-      <c r="E18" s="1" t="n"/>
-      <c r="F18" s="1" t="n"/>
-    </row>
-    <row r="19" ht="20" customHeight="1">
+      <c r="B18" s="2" t="n"/>
+      <c r="C18" s="2" t="n"/>
+      <c r="D18" s="2" t="n"/>
+      <c r="E18" s="2" t="n"/>
+      <c r="F18" s="2" t="n"/>
+    </row>
+    <row r="19" ht="30" customHeight="1">
       <c r="A19" s="1" t="inlineStr">
         <is>
           <t>4:30 p.m.</t>
         </is>
       </c>
-      <c r="B19" s="1" t="n"/>
-      <c r="C19" s="1" t="n"/>
-      <c r="D19" s="1" t="n"/>
-      <c r="E19" s="1" t="n"/>
-      <c r="F19" s="1" t="n"/>
-    </row>
-    <row r="20" ht="20" customHeight="1">
+      <c r="B19" s="2" t="n"/>
+      <c r="C19" s="2" t="n"/>
+      <c r="D19" s="2" t="n"/>
+      <c r="E19" s="2" t="n"/>
+      <c r="F19" s="2" t="n"/>
+    </row>
+    <row r="20" ht="30" customHeight="1">
       <c r="A20" s="1" t="inlineStr">
         <is>
           <t>5:00 p.m.</t>
         </is>
       </c>
-      <c r="B20" s="1" t="n"/>
-      <c r="C20" s="1" t="inlineStr">
-        <is>
-          <t>CPSC_V 330-103 - Applied Machine Learning
-5:00 p.m. - 6:30 p.m.</t>
-        </is>
-      </c>
-      <c r="D20" s="1" t="n"/>
-      <c r="E20" s="1" t="inlineStr">
-        <is>
-          <t>CPSC_V 330-103 - Applied Machine Learning
-5:00 p.m. - 6:30 p.m.</t>
-        </is>
-      </c>
-      <c r="F20" s="1" t="n"/>
-    </row>
-    <row r="21" ht="20" customHeight="1">
+      <c r="B20" s="2" t="n"/>
+      <c r="C20" s="2" t="n"/>
+      <c r="D20" s="2" t="n"/>
+      <c r="E20" s="2" t="n"/>
+      <c r="F20" s="2" t="n"/>
+    </row>
+    <row r="21" ht="30" customHeight="1">
       <c r="A21" s="1" t="inlineStr">
         <is>
           <t>5:30 p.m.</t>
         </is>
       </c>
-      <c r="B21" s="1" t="n"/>
-      <c r="C21" s="1" t="n"/>
-      <c r="D21" s="1" t="n"/>
-      <c r="E21" s="1" t="n"/>
-      <c r="F21" s="1" t="n"/>
-    </row>
-    <row r="22" ht="20" customHeight="1">
+      <c r="B21" s="2" t="n"/>
+      <c r="C21" s="2" t="n"/>
+      <c r="D21" s="2" t="n"/>
+      <c r="E21" s="2" t="n"/>
+      <c r="F21" s="2" t="n"/>
+    </row>
+    <row r="22" ht="30" customHeight="1">
       <c r="A22" s="1" t="inlineStr">
         <is>
           <t>6:00 p.m.</t>
         </is>
       </c>
-      <c r="B22" s="1" t="n"/>
-      <c r="C22" s="1" t="n"/>
-      <c r="D22" s="1" t="n"/>
-      <c r="E22" s="1" t="n"/>
-      <c r="F22" s="1" t="n"/>
-    </row>
-    <row r="23" ht="20" customHeight="1">
+      <c r="B22" s="2" t="n"/>
+      <c r="C22" s="2" t="n"/>
+      <c r="D22" s="2" t="n"/>
+      <c r="E22" s="2" t="n"/>
+      <c r="F22" s="2" t="n"/>
+    </row>
+    <row r="23" ht="30" customHeight="1">
       <c r="A23" s="1" t="inlineStr">
         <is>
           <t>6:30 p.m.</t>
         </is>
       </c>
-      <c r="B23" s="1" t="n"/>
-      <c r="C23" s="1" t="n"/>
-      <c r="D23" s="1" t="n"/>
-      <c r="E23" s="1" t="n"/>
-      <c r="F23" s="1" t="n"/>
-    </row>
-    <row r="24" ht="20" customHeight="1">
+      <c r="B23" s="2" t="n"/>
+      <c r="C23" s="2" t="n"/>
+      <c r="D23" s="2" t="n"/>
+      <c r="E23" s="2" t="n"/>
+      <c r="F23" s="2" t="n"/>
+    </row>
+    <row r="24" ht="30" customHeight="1">
       <c r="A24" s="1" t="inlineStr">
         <is>
           <t>7:00 p.m.</t>
         </is>
       </c>
-      <c r="B24" s="1" t="n"/>
-      <c r="C24" s="1" t="n"/>
-      <c r="D24" s="1" t="n"/>
-      <c r="E24" s="1" t="n"/>
-      <c r="F24" s="1" t="n"/>
-    </row>
-    <row r="25" ht="20" customHeight="1">
+      <c r="B24" s="2" t="n"/>
+      <c r="C24" s="2" t="n"/>
+      <c r="D24" s="2" t="n"/>
+      <c r="E24" s="2" t="n"/>
+      <c r="F24" s="2" t="n"/>
+    </row>
+    <row r="25" ht="30" customHeight="1">
       <c r="A25" s="1" t="inlineStr">
         <is>
           <t>7:30 p.m.</t>
         </is>
       </c>
-      <c r="B25" s="1" t="n"/>
-      <c r="C25" s="1" t="n"/>
-      <c r="D25" s="1" t="n"/>
-      <c r="E25" s="1" t="n"/>
-      <c r="F25" s="1" t="n"/>
-    </row>
-    <row r="26" ht="20" customHeight="1">
+      <c r="B25" s="2" t="n"/>
+      <c r="C25" s="2" t="n"/>
+      <c r="D25" s="2" t="n"/>
+      <c r="E25" s="2" t="n"/>
+      <c r="F25" s="2" t="n"/>
+    </row>
+    <row r="26" ht="30" customHeight="1">
       <c r="A26" s="1" t="inlineStr">
         <is>
           <t>8:00 p.m.</t>
         </is>
       </c>
-      <c r="B26" s="1" t="n"/>
-      <c r="C26" s="1" t="n"/>
-      <c r="D26" s="1" t="n"/>
-      <c r="E26" s="1" t="n"/>
-      <c r="F26" s="1" t="n"/>
-    </row>
-    <row r="27" ht="20" customHeight="1">
+      <c r="B26" s="2" t="n"/>
+      <c r="C26" s="2" t="n"/>
+      <c r="D26" s="2" t="n"/>
+      <c r="E26" s="2" t="n"/>
+      <c r="F26" s="2" t="n"/>
+    </row>
+    <row r="27" ht="30" customHeight="1">
       <c r="A27" s="1" t="inlineStr">
         <is>
           <t>8:30 p.m.</t>
         </is>
       </c>
-      <c r="B27" s="1" t="n"/>
-      <c r="C27" s="1" t="n"/>
-      <c r="D27" s="1" t="n"/>
-      <c r="E27" s="1" t="n"/>
-      <c r="F27" s="1" t="n"/>
-    </row>
-    <row r="28" ht="20" customHeight="1">
+      <c r="B27" s="2" t="n"/>
+      <c r="C27" s="2" t="n"/>
+      <c r="D27" s="2" t="n"/>
+      <c r="E27" s="2" t="n"/>
+      <c r="F27" s="2" t="n"/>
+    </row>
+    <row r="28" ht="30" customHeight="1">
       <c r="A28" s="1" t="inlineStr">
         <is>
           <t>9:00 p.m.</t>
         </is>
       </c>
-      <c r="B28" s="1" t="n"/>
-      <c r="C28" s="1" t="n"/>
-      <c r="D28" s="1" t="n"/>
-      <c r="E28" s="1" t="n"/>
-      <c r="F28" s="1" t="n"/>
-    </row>
-    <row r="29" ht="20" customHeight="1">
+      <c r="B28" s="2" t="n"/>
+      <c r="C28" s="2" t="n"/>
+      <c r="D28" s="2" t="n"/>
+      <c r="E28" s="2" t="n"/>
+      <c r="F28" s="2" t="n"/>
+    </row>
+    <row r="29" ht="30" customHeight="1">
       <c r="A29" s="1" t="inlineStr">
         <is>
           <t>9:30 p.m.</t>
         </is>
       </c>
-      <c r="B29" s="1" t="n"/>
-      <c r="C29" s="1" t="n"/>
-      <c r="D29" s="1" t="n"/>
-      <c r="E29" s="1" t="n"/>
-      <c r="F29" s="1" t="n"/>
+      <c r="B29" s="2" t="n"/>
+      <c r="C29" s="2" t="n"/>
+      <c r="D29" s="2" t="n"/>
+      <c r="E29" s="2" t="n"/>
+      <c r="F29" s="2" t="n"/>
     </row>
     <row r="30">
-      <c r="A30" t="inlineStr">
+      <c r="A30" s="1" t="inlineStr">
         <is>
           <t>10:00 p.m.</t>
         </is>
       </c>
+      <c r="B30" s="2" t="n"/>
+      <c r="C30" s="2" t="n"/>
+      <c r="D30" s="2" t="n"/>
+      <c r="E30" s="2" t="n"/>
+      <c r="F30" s="2" t="n"/>
     </row>
   </sheetData>
   <mergeCells count="10">
-    <mergeCell ref="E8:E10"/>
-    <mergeCell ref="B4:B7"/>
-    <mergeCell ref="E12:E13"/>
-    <mergeCell ref="C20:C22"/>
-    <mergeCell ref="E20:E22"/>
-    <mergeCell ref="E2:E7"/>
-    <mergeCell ref="C8:C10"/>
-    <mergeCell ref="D14:D15"/>
-    <mergeCell ref="B14:B15"/>
-    <mergeCell ref="F14:F15"/>
+    <mergeCell ref="F8:F9"/>
+    <mergeCell ref="B12:B13"/>
+    <mergeCell ref="F12:F13"/>
+    <mergeCell ref="C11:C13"/>
+    <mergeCell ref="D8:D9"/>
+    <mergeCell ref="B8:B9"/>
+    <mergeCell ref="E11:E13"/>
+    <mergeCell ref="E6:E7"/>
+    <mergeCell ref="C6:C7"/>
+    <mergeCell ref="D12:D13"/>
   </mergeCells>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Created error messages that pop up when users upload the wrong files onto the website and also designed the website to become more user oriented.
</commit_message>
<xml_diff>
--- a/new-schedule.xlsx
+++ b/new-schedule.xlsx
@@ -496,7 +496,12 @@
       </c>
       <c r="B4" s="2" t="n"/>
       <c r="C4" s="2" t="n"/>
-      <c r="D4" s="2" t="n"/>
+      <c r="D4" s="2" t="inlineStr">
+        <is>
+          <t>CPSC_V 221-L1K - Basic Algorithms and Data Structures
+9:00 a.m. - 11:00 a.m.</t>
+        </is>
+      </c>
       <c r="E4" s="2" t="n"/>
       <c r="F4" s="2" t="n"/>
     </row>
@@ -507,9 +512,19 @@
         </is>
       </c>
       <c r="B5" s="2" t="n"/>
-      <c r="C5" s="2" t="n"/>
+      <c r="C5" s="2" t="inlineStr">
+        <is>
+          <t>ENGL_V 111-002 - Approaches to Language and Communication
+9:30 a.m. - 11:00 a.m.</t>
+        </is>
+      </c>
       <c r="D5" s="2" t="n"/>
-      <c r="E5" s="2" t="n"/>
+      <c r="E5" s="2" t="inlineStr">
+        <is>
+          <t>ENGL_V 111-L10 - Approaches to Language and Communication
+9:30 a.m. - 11:00 a.m.</t>
+        </is>
+      </c>
       <c r="F5" s="2" t="n"/>
     </row>
     <row r="6" ht="30" customHeight="1">
@@ -519,19 +534,9 @@
         </is>
       </c>
       <c r="B6" s="2" t="n"/>
-      <c r="C6" s="2" t="inlineStr">
-        <is>
-          <t>CPSC_V 213-L2F - Introduction to Computer Systems
-10:00 a.m. - 11:00 a.m.</t>
-        </is>
-      </c>
+      <c r="C6" s="2" t="n"/>
       <c r="D6" s="2" t="n"/>
-      <c r="E6" s="2" t="inlineStr">
-        <is>
-          <t>CPSC_V 213-L2F - Introduction to Computer Systems
-10:00 a.m. - 11:00 a.m.</t>
-        </is>
-      </c>
+      <c r="E6" s="2" t="n"/>
       <c r="F6" s="2" t="n"/>
     </row>
     <row r="7" ht="30" customHeight="1">
@@ -552,26 +557,21 @@
           <t>11:00 a.m.</t>
         </is>
       </c>
-      <c r="B8" s="2" t="inlineStr">
-        <is>
-          <t>CPSC_V 213-205 - Introduction to Computer Systems
-11:00 a.m. - 12:00 p.m.</t>
-        </is>
-      </c>
-      <c r="C8" s="2" t="n"/>
-      <c r="D8" s="2" t="inlineStr">
-        <is>
-          <t>CPSC_V 213-205 - Introduction to Computer Systems
-11:00 a.m. - 12:00 p.m.</t>
-        </is>
-      </c>
-      <c r="E8" s="2" t="n"/>
-      <c r="F8" s="2" t="inlineStr">
-        <is>
-          <t>CPSC_V 213-205 - Introduction to Computer Systems
-11:00 a.m. - 12:00 p.m.</t>
-        </is>
-      </c>
+      <c r="B8" s="2" t="n"/>
+      <c r="C8" s="2" t="inlineStr">
+        <is>
+          <t>MATH_V 200-102 - Calculus III
+11:00 a.m. - 12:30 p.m.</t>
+        </is>
+      </c>
+      <c r="D8" s="2" t="n"/>
+      <c r="E8" s="2" t="inlineStr">
+        <is>
+          <t>MATH_V 200-102 - Calculus III
+11:00 a.m. - 12:30 p.m.</t>
+        </is>
+      </c>
+      <c r="F8" s="2" t="n"/>
     </row>
     <row r="9" ht="30" customHeight="1">
       <c r="A9" s="1" t="inlineStr">
@@ -604,19 +604,9 @@
         </is>
       </c>
       <c r="B11" s="2" t="n"/>
-      <c r="C11" s="2" t="inlineStr">
-        <is>
-          <t>MATH_V 221-202 - Matrix Algebra
-12:30 p.m. - 2:00 p.m.</t>
-        </is>
-      </c>
+      <c r="C11" s="2" t="n"/>
       <c r="D11" s="2" t="n"/>
-      <c r="E11" s="2" t="inlineStr">
-        <is>
-          <t>MATH_V 221-202 - Matrix Algebra
-12:30 p.m. - 2:00 p.m.</t>
-        </is>
-      </c>
+      <c r="E11" s="2" t="n"/>
       <c r="F11" s="2" t="n"/>
     </row>
     <row r="12" ht="30" customHeight="1">
@@ -625,26 +615,16 @@
           <t>1:00 p.m.</t>
         </is>
       </c>
-      <c r="B12" s="2" t="inlineStr">
-        <is>
-          <t>ENGL_V 110-010 - Approaches to Literature and Culture
+      <c r="B12" s="2" t="n"/>
+      <c r="C12" s="2" t="n"/>
+      <c r="D12" s="2" t="n"/>
+      <c r="E12" s="2" t="inlineStr">
+        <is>
+          <t>CPSC_V 330-T1F - Applied Machine Learning
 1:00 p.m. - 2:00 p.m.</t>
         </is>
       </c>
-      <c r="C12" s="2" t="n"/>
-      <c r="D12" s="2" t="inlineStr">
-        <is>
-          <t>ENGL_V 110-010 - Approaches to Literature and Culture
-1:00 p.m. - 2:00 p.m.</t>
-        </is>
-      </c>
-      <c r="E12" s="2" t="n"/>
-      <c r="F12" s="2" t="inlineStr">
-        <is>
-          <t>ENGL_V 110-LS1 - Approaches to Literature and Culture
-1:00 p.m. - 2:00 p.m.</t>
-        </is>
-      </c>
+      <c r="F12" s="2" t="n"/>
     </row>
     <row r="13" ht="30" customHeight="1">
       <c r="A13" s="1" t="inlineStr">
@@ -664,11 +644,26 @@
           <t>2:00 p.m.</t>
         </is>
       </c>
-      <c r="B14" s="2" t="n"/>
+      <c r="B14" s="2" t="inlineStr">
+        <is>
+          <t>CPSC_V 221-101 - Basic Algorithms and Data Structures
+2:00 p.m. - 3:00 p.m.</t>
+        </is>
+      </c>
       <c r="C14" s="2" t="n"/>
-      <c r="D14" s="2" t="n"/>
+      <c r="D14" s="2" t="inlineStr">
+        <is>
+          <t>CPSC_V 221-101 - Basic Algorithms and Data Structures
+2:00 p.m. - 3:00 p.m.</t>
+        </is>
+      </c>
       <c r="E14" s="2" t="n"/>
-      <c r="F14" s="2" t="n"/>
+      <c r="F14" s="2" t="inlineStr">
+        <is>
+          <t>CPSC_V 221-101 - Basic Algorithms and Data Structures
+2:00 p.m. - 3:00 p.m.</t>
+        </is>
+      </c>
     </row>
     <row r="15" ht="30" customHeight="1">
       <c r="A15" s="1" t="inlineStr">
@@ -701,9 +696,19 @@
         </is>
       </c>
       <c r="B17" s="2" t="n"/>
-      <c r="C17" s="2" t="n"/>
+      <c r="C17" s="2" t="inlineStr">
+        <is>
+          <t>CPSC_V 330-101 - Applied Machine Learning
+3:30 p.m. - 5:00 p.m.</t>
+        </is>
+      </c>
       <c r="D17" s="2" t="n"/>
-      <c r="E17" s="2" t="n"/>
+      <c r="E17" s="2" t="inlineStr">
+        <is>
+          <t>CPSC_V 330-101 - Applied Machine Learning
+3:30 p.m. - 5:00 p.m.</t>
+        </is>
+      </c>
       <c r="F17" s="2" t="n"/>
     </row>
     <row r="18" ht="30" customHeight="1">
@@ -863,17 +868,18 @@
       <c r="F30" s="2" t="n"/>
     </row>
   </sheetData>
-  <mergeCells count="10">
-    <mergeCell ref="F8:F9"/>
-    <mergeCell ref="B12:B13"/>
-    <mergeCell ref="F12:F13"/>
-    <mergeCell ref="C11:C13"/>
-    <mergeCell ref="D8:D9"/>
-    <mergeCell ref="B8:B9"/>
-    <mergeCell ref="E11:E13"/>
-    <mergeCell ref="E6:E7"/>
-    <mergeCell ref="C6:C7"/>
-    <mergeCell ref="D12:D13"/>
+  <mergeCells count="11">
+    <mergeCell ref="D4:D7"/>
+    <mergeCell ref="E17:E19"/>
+    <mergeCell ref="E8:E10"/>
+    <mergeCell ref="E12:E13"/>
+    <mergeCell ref="C17:C19"/>
+    <mergeCell ref="C5:C7"/>
+    <mergeCell ref="E5:E7"/>
+    <mergeCell ref="C8:C10"/>
+    <mergeCell ref="D14:D15"/>
+    <mergeCell ref="B14:B15"/>
+    <mergeCell ref="F14:F15"/>
   </mergeCells>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>